<commit_message>
Finish Delete Question by ID and Section
</commit_message>
<xml_diff>
--- a/backend/src/data/dummy_questions/dummy_akudak.xlsx
+++ b/backend/src/data/dummy_questions/dummy_akudak.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\dummy_questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A5D052-DCD8-4549-94AF-F4BC9D8FB9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A50CD3-DF64-4A0B-BAA8-64ADC0BB4A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="754" activeTab="2" xr2:uid="{1C76B0C7-30FC-44AF-999C-E5F402443C8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="754" xr2:uid="{1C76B0C7-30FC-44AF-999C-E5F402443C8E}"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="Soal" sheetId="1" r:id="rId1"/>
     <sheet name="2" sheetId="6" r:id="rId2"/>
     <sheet name="3" sheetId="7" r:id="rId3"/>
     <sheet name="4" sheetId="8" r:id="rId4"/>
@@ -766,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1252DDF0-61D8-4308-9257-82AA9345D5F2}">
   <dimension ref="A1:L156"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
@@ -6160,7 +6160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D70B9DE-8B62-44E7-B392-989C4BF942C0}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>

</xml_diff>